<commit_message>
externalize popup content into content.csv
</commit_message>
<xml_diff>
--- a/etc/post-storm-content.xlsx
+++ b/etc/post-storm-content.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>key</t>
   </si>
@@ -80,6 +80,42 @@
   </si>
   <si>
     <t>shelter</t>
+  </si>
+  <si>
+    <t>user_in_x_zone</t>
+  </si>
+  <si>
+    <t>user_zone_unkown</t>
+  </si>
+  <si>
+    <t>user_zone_unkown_311</t>
+  </si>
+  <si>
+    <t>user_zone</t>
+  </si>
+  <si>
+    <t>evac_order</t>
+  </si>
+  <si>
+    <t>no_evac_order</t>
+  </si>
+  <si>
+    <t>You are not located in an Evacuation Zone (post-storm)</t>
+  </si>
+  <si>
+    <t>Zone Finder cannot determine Zone for your address.&lt;br&gt;Try alternative address or determine Zone by examining map and clicking on your location. (post-storm)</t>
+  </si>
+  <si>
+    <t>Zone Finder cannot determine Zone for your address.&lt;br&gt;Try alternative address. (post-storm)</t>
+  </si>
+  <si>
+    <t>You are located in Zone ${zone} (post-storm)</t>
+  </si>
+  <si>
+    <t>You are required to evacuate (post-storm)</t>
+  </si>
+  <si>
+    <t>No evacuation order currently in effect (post-storm)</t>
   </si>
 </sst>
 </file>
@@ -924,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,8 +1051,56 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yhxeFKXQSv0/Pnw3xBJ4nLYh1fKrZFzO7ZWhpfL0CS3BipMyAaRFmCLudnVhkiuiWciLvPOvPnxNw9ixmzriyw==" saltValue="MLHPIcHEQMClU6/dH5n7aQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="99lSHNn6n7CHTyTK0OsYSVP5Rr++9ml2BeZxmVJK1qaydxErhqF4X+w6Q7II14fNgnFbEjPTgzc+PpO4TKp48Q==" saltValue="Z7YmZxtxbIpJIOHkwXy5wA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
somewhat representative post-storm content as per oem
</commit_message>
<xml_diff>
--- a/etc/post-storm-content.xlsx
+++ b/etc/post-storm-content.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkeane\git\hurricane\etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\git\hurricane\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="4605"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ESRI_MAPINFO_SHEET" sheetId="3" state="veryHidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>key</t>
   </si>
@@ -61,24 +62,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Something different</t>
-  </si>
-  <si>
-    <t>A different splash message</t>
-  </si>
-  <si>
-    <t>Lookie a map</t>
-  </si>
-  <si>
-    <t>shelters</t>
-  </si>
-  <si>
-    <t>A different centers message</t>
-  </si>
-  <si>
-    <t>A different legend message</t>
-  </si>
-  <si>
     <t>shelter</t>
   </si>
   <si>
@@ -100,22 +83,34 @@
     <t>no_evac_order</t>
   </si>
   <si>
-    <t>You are not located in an Evacuation Zone (post-storm)</t>
-  </si>
-  <si>
-    <t>Zone Finder cannot determine Zone for your address.&lt;br&gt;Try alternative address or determine Zone by examining map and clicking on your location. (post-storm)</t>
-  </si>
-  <si>
-    <t>Zone Finder cannot determine Zone for your address.&lt;br&gt;Try alternative address. (post-storm)</t>
-  </si>
-  <si>
-    <t>You are located in Zone ${zone} (post-storm)</t>
-  </si>
-  <si>
-    <t>You are required to evacuate (post-storm)</t>
-  </si>
-  <si>
-    <t>No evacuation order currently in effect (post-storm)</t>
+    <t>Hurricane Josh Shelter Locator</t>
+  </si>
+  <si>
+    <t>If you need emergency shelter as a result of Hurricane Josh, use the map to find the nearest facility or call 311 for info</t>
+  </si>
+  <si>
+    <t>Shelter Map</t>
+  </si>
+  <si>
+    <t>Shelters</t>
+  </si>
+  <si>
+    <t>Areas impacted by Hurricane Josh may still be unsafe. If you cannot remain in your home, use this application or call 311 to located a city-operated shelter.</t>
+  </si>
+  <si>
+    <t>If your home is unsafe, you may go to one of the shelters listed below. If you cannot get there on your own please call 311. CHECK BACK DAILY AS THE LIST OF SHELTERS MAY CHANGE</t>
+  </si>
+  <si>
+    <t>You are not located in an area impaced by Hurricane Josh storm surge</t>
+  </si>
+  <si>
+    <t>Zone Finder cannot determine your address.&lt;br&gt;Try alternative address or examine map and click on your location.</t>
+  </si>
+  <si>
+    <t>Zone Finder cannot determine your address.&lt;br&gt;Try alternative address.</t>
+  </si>
+  <si>
+    <t>You are in an area that may have been impacted by Hurricane Josh</t>
   </si>
 </sst>
 </file>
@@ -661,6 +656,100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>294147</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>126965</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="EsriDoNotEdit"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6390147" cy="1650965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>DO NOT EDIT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> For Esri use only</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -963,7 +1052,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +1081,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1000,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1008,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1016,7 +1105,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1024,7 +1113,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,7 +1121,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1040,7 +1129,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,12 +1137,12 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
@@ -1061,7 +1150,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>27</v>
@@ -1069,7 +1158,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>28</v>
@@ -1077,27 +1166,25 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B16" s="2"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="t23QBdSrII4Pz+W5TnO/70GfpSRpzw4V43LxmdchNmFcjpE/nPcd419l02BWHaBZBK+ZYEFYgGc3ZDq3Ey119A==" saltValue="rsRA2GjslSKY1cTJ8a9yWA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -1142,4 +1229,17 @@
   <sheetProtection algorithmName="SHA-512" hashValue="3VOf/Jl/LcaHMm9RRzyQFMmUJdOCtSrWkk8A5QEOWpyV7pd6JiOqRLg3rlQmU4WuOgd7EA01tREJH7TsmkFGVA==" saltValue="IlQm4E2xL7/t+QKqHHg/Pg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>